<commit_message>
minor changes at backend
</commit_message>
<xml_diff>
--- a/BridgeCareApp/BridgeCareCore/DownloadTemplates/TreatmentSupersedeRules_template.xlsx
+++ b/BridgeCareApp/BridgeCareCore/DownloadTemplates/TreatmentSupersedeRules_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aborgaonkar\source\repos\Infrastructure Asset Management\BridgeCareApp\BridgeCareCore\DownloadTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{890683E9-0A72-46A1-A8DE-0E3BB3282A23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9A94F93-CD71-4BA6-AD3C-E1F9059CBE63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,15 +35,21 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -66,9 +72,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -391,14 +402,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="58.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="51.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="40.7109375" customWidth="1"/>
     <col min="4" max="4" width="80" customWidth="1"/>
     <col min="5" max="9" width="40" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="23.25">
+    <row r="1" spans="1:3" s="2" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -411,5 +420,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>